<commit_message>
updated a digikey part num
</commit_message>
<xml_diff>
--- a/hardware/squall/rev_a/squall_bom.xlsx
+++ b/hardware/squall/rev_a/squall_bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="108" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="99" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,6 +27,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">This is for 250, waiting on a 1000 quote</t>
         </r>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="140">
   <si>
     <t>Qty</t>
   </si>
@@ -156,31 +157,34 @@
     <t>0402 Capacitor</t>
   </si>
   <si>
+    <t>490-6269-1-ND</t>
+  </si>
+  <si>
+    <t>12pF</t>
+  </si>
+  <si>
+    <t>C2, C3, C4, C5</t>
+  </si>
+  <si>
+    <t>490-6197-1-ND</t>
+  </si>
+  <si>
+    <t>1nF</t>
+  </si>
+  <si>
+    <t>C6, C7</t>
+  </si>
+  <si>
+    <t>490-1303-1-ND</t>
+  </si>
+  <si>
+    <t>2.2nF</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
     <t>490-5419-1-ND</t>
-  </si>
-  <si>
-    <t>12pF</t>
-  </si>
-  <si>
-    <t>C2, C3, C4, C5</t>
-  </si>
-  <si>
-    <t>490-6197-1-ND</t>
-  </si>
-  <si>
-    <t>1nF</t>
-  </si>
-  <si>
-    <t>C6, C7</t>
-  </si>
-  <si>
-    <t>490-1303-1-ND</t>
-  </si>
-  <si>
-    <t>2.2nF</t>
-  </si>
-  <si>
-    <t>C8</t>
   </si>
   <si>
     <t>47nF</t>
@@ -468,6 +472,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -489,6 +494,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -588,7 +594,7 @@
   <dimension ref="1:31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M31" activeCellId="0" sqref="M31"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -957,7 +963,7 @@
         <v>38</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="K9" s="0" t="n">
         <v>0.0127</v>
@@ -982,7 +988,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>35</v>
@@ -991,13 +997,13 @@
         <v>36</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>38</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K10" s="0" t="n">
         <v>0.0151</v>
@@ -1022,7 +1028,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>35</v>
@@ -1031,13 +1037,13 @@
         <v>36</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>38</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>0.0136</v>
@@ -1062,7 +1068,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>35</v>
@@ -1071,13 +1077,13 @@
         <v>36</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>38</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>0.01</v>
@@ -1099,7 +1105,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>35</v>
@@ -1108,13 +1114,13 @@
         <v>36</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>38</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>0.058</v>
@@ -1136,7 +1142,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>35</v>
@@ -1145,13 +1151,13 @@
         <v>36</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>38</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>0.122</v>
@@ -1173,22 +1179,22 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>0.0925</v>
@@ -1213,25 +1219,25 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>0.11</v>
@@ -1253,28 +1259,28 @@
         <v>2</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K17" s="0" t="n">
         <v>0.38815</v>
@@ -1299,25 +1305,25 @@
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K18" s="0" t="n">
         <v>0.60558</v>
@@ -1339,22 +1345,22 @@
         <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>36</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>0.034</v>
@@ -1379,22 +1385,22 @@
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K20" s="0" t="n">
         <v>0.07434</v>
@@ -1419,19 +1425,19 @@
         <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>36</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K21" s="0" t="n">
         <v>0.0334</v>
@@ -1456,19 +1462,19 @@
         <v>150</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K22" s="0" t="n">
         <v>0.00933</v>
@@ -1490,22 +1496,22 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K23" s="0" t="n">
         <v>0.00933</v>
@@ -1530,22 +1536,22 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K24" s="0" t="n">
         <v>0.00933</v>
@@ -1570,22 +1576,22 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K25" s="0" t="n">
         <v>0.66414</v>
@@ -1607,22 +1613,22 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K26" s="0" t="n">
         <v>2.31</v>
@@ -1647,25 +1653,25 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K27" s="0" t="n">
         <v>3.301</v>
@@ -1687,22 +1693,22 @@
         <v>1</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K28" s="0" t="n">
         <v>0.782</v>
@@ -1727,22 +1733,22 @@
         <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K29" s="0" t="n">
         <v>1.061</v>
@@ -1761,10 +1767,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F30" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K30" s="0" t="n">
         <v>0.15579</v>

</xml_diff>